<commit_message>
backup to prod branch, merging prod and master after security fixes
</commit_message>
<xml_diff>
--- a/reporting/scoutapp/utils/Scouting-Report-Temp.xlsx
+++ b/reporting/scoutapp/utils/Scouting-Report-Temp.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="206">
   <si>
     <t>Psyllid Scouting Report</t>
   </si>
@@ -228,9 +228,6 @@
   </si>
   <si>
     <t>53 D 1 (West)</t>
-  </si>
-  <si>
-    <t>2017-04-05</t>
   </si>
   <si>
     <t>53 D 2 (East)</t>
@@ -575,9 +572,6 @@
     <t>Lime/Lemon</t>
   </si>
   <si>
-    <t>2017-04-04</t>
-  </si>
-  <si>
     <t>Total number of Young blocks:</t>
   </si>
   <si>
@@ -638,19 +632,10 @@
     <t>U5B</t>
   </si>
   <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>low</t>
+    <t>120 D Young</t>
   </si>
   <si>
     <t>high</t>
-  </si>
-  <si>
-    <t>120 D Young</t>
   </si>
 </sst>
 </file>
@@ -1484,7 +1469,7 @@
   <dimension ref="A1:AE278"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" zoomScale="60" zoomScaleNormal="71" zoomScalePageLayoutView="71">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F10" sqref="F10:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="0"/>
@@ -2023,8 +2008,9 @@
         <f>IF('Mature Data'!F9="","",'Mature Data'!F9)</f>
         <v/>
       </c>
-      <c r="G10" s="25" t="n">
-        <v>8</v>
+      <c r="G10" s="25">
+        <f>IF('Mature Data'!G9="","",'Mature Data'!G9)</f>
+        <v/>
       </c>
       <c r="H10" s="25">
         <f>IF('Mature Data'!H9="","",'Mature Data'!H9)</f>
@@ -58893,76 +58879,10 @@
       <c r="B21" t="s">
         <v>55</v>
       </c>
-      <c r="D21" t="s">
-        <v>70</v>
-      </c>
-      <c r="G21" t="n">
-        <v>0</v>
-      </c>
-      <c r="H21" t="n">
-        <v>0</v>
-      </c>
-      <c r="I21" t="n">
-        <v>2</v>
-      </c>
-      <c r="M21" t="n">
-        <v>1</v>
-      </c>
-      <c r="N21" t="n">
-        <v>7</v>
-      </c>
-      <c r="O21" t="n">
-        <v>7</v>
-      </c>
-      <c r="S21" t="n">
-        <v>0</v>
-      </c>
-      <c r="T21" t="n">
-        <v>0</v>
-      </c>
-      <c r="U21" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y21" t="n">
-        <v>5</v>
-      </c>
-      <c r="Z21" t="n">
-        <v>10</v>
-      </c>
-      <c r="AA21" t="n">
-        <v>13</v>
-      </c>
-      <c r="AE21" t="s">
-        <v>51</v>
-      </c>
-      <c r="AF21" t="s">
-        <v>51</v>
-      </c>
-      <c r="AG21" t="s">
-        <v>51</v>
-      </c>
-      <c r="AK21" t="s">
-        <v>51</v>
-      </c>
-      <c r="AL21" t="s">
-        <v>51</v>
-      </c>
-      <c r="AM21" t="s">
-        <v>51</v>
-      </c>
-      <c r="AQ21" t="s">
-        <v>51</v>
-      </c>
-      <c r="AR21" t="s">
-        <v>51</v>
-      </c>
-      <c r="AS21" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="22" spans="1:45">
       <c r="A22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B22" t="s">
         <v>55</v>
@@ -58970,408 +58890,42 @@
     </row>
     <row r="23" spans="1:45">
       <c r="A23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B23" t="s">
         <v>55</v>
       </c>
-      <c r="D23" t="s">
-        <v>70</v>
-      </c>
-      <c r="E23" t="n">
-        <v>1</v>
-      </c>
-      <c r="F23" t="n">
-        <v>1</v>
-      </c>
-      <c r="G23" t="n">
-        <v>0</v>
-      </c>
-      <c r="H23" t="n">
-        <v>0</v>
-      </c>
-      <c r="I23" t="n">
-        <v>0</v>
-      </c>
-      <c r="K23" t="n">
-        <v>2</v>
-      </c>
-      <c r="L23" t="n">
-        <v>5</v>
-      </c>
-      <c r="M23" t="n">
-        <v>2</v>
-      </c>
-      <c r="N23" t="n">
-        <v>9</v>
-      </c>
-      <c r="O23" t="n">
-        <v>8</v>
-      </c>
-      <c r="Q23" t="n">
-        <v>0</v>
-      </c>
-      <c r="R23" t="n">
-        <v>0</v>
-      </c>
-      <c r="S23" t="n">
-        <v>0</v>
-      </c>
-      <c r="T23" t="n">
-        <v>0</v>
-      </c>
-      <c r="U23" t="n">
-        <v>0</v>
-      </c>
-      <c r="W23" t="n">
-        <v>12</v>
-      </c>
-      <c r="X23" t="n">
-        <v>10</v>
-      </c>
-      <c r="Y23" t="n">
-        <v>10</v>
-      </c>
-      <c r="Z23" t="n">
-        <v>16</v>
-      </c>
-      <c r="AA23" t="n">
-        <v>15</v>
-      </c>
-      <c r="AC23" t="s">
-        <v>51</v>
-      </c>
-      <c r="AD23" t="s">
-        <v>51</v>
-      </c>
-      <c r="AE23" t="s">
-        <v>51</v>
-      </c>
-      <c r="AF23" t="s">
-        <v>51</v>
-      </c>
-      <c r="AG23" t="s">
-        <v>51</v>
-      </c>
-      <c r="AI23" t="s">
-        <v>51</v>
-      </c>
-      <c r="AJ23" t="s">
-        <v>51</v>
-      </c>
-      <c r="AK23" t="s">
-        <v>51</v>
-      </c>
-      <c r="AL23" t="s">
-        <v>51</v>
-      </c>
-      <c r="AM23" t="s">
-        <v>51</v>
-      </c>
-      <c r="AO23" t="s">
-        <v>51</v>
-      </c>
-      <c r="AP23" t="s">
-        <v>51</v>
-      </c>
-      <c r="AQ23" t="s">
-        <v>51</v>
-      </c>
-      <c r="AR23" t="s">
-        <v>51</v>
-      </c>
       <c r="AS23" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:45">
       <c r="A24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B24" t="s">
         <v>55</v>
       </c>
-      <c r="D24" t="s">
-        <v>70</v>
-      </c>
-      <c r="E24" t="n">
-        <v>0</v>
-      </c>
-      <c r="F24" t="n">
-        <v>1</v>
-      </c>
-      <c r="G24" t="n">
-        <v>0</v>
-      </c>
-      <c r="H24" t="n">
-        <v>1</v>
-      </c>
-      <c r="I24" t="n">
-        <v>0</v>
-      </c>
-      <c r="K24" t="n">
-        <v>6</v>
-      </c>
-      <c r="L24" t="n">
-        <v>4</v>
-      </c>
-      <c r="M24" t="n">
-        <v>1</v>
-      </c>
-      <c r="N24" t="n">
-        <v>3</v>
-      </c>
-      <c r="O24" t="n">
-        <v>6</v>
-      </c>
-      <c r="Q24" t="n">
-        <v>0</v>
-      </c>
-      <c r="R24" t="n">
-        <v>0</v>
-      </c>
-      <c r="S24" t="n">
-        <v>0</v>
-      </c>
-      <c r="T24" t="n">
-        <v>0</v>
-      </c>
-      <c r="U24" t="n">
-        <v>0</v>
-      </c>
-      <c r="W24" t="n">
-        <v>6</v>
-      </c>
-      <c r="X24" t="n">
-        <v>7</v>
-      </c>
-      <c r="Y24" t="n">
-        <v>3</v>
-      </c>
-      <c r="Z24" t="n">
-        <v>7</v>
-      </c>
-      <c r="AA24" t="n">
-        <v>11</v>
-      </c>
-      <c r="AC24" t="s">
-        <v>51</v>
-      </c>
-      <c r="AD24" t="s">
-        <v>51</v>
-      </c>
-      <c r="AE24" t="s">
-        <v>51</v>
-      </c>
-      <c r="AF24" t="s">
-        <v>51</v>
-      </c>
-      <c r="AG24" t="s">
-        <v>51</v>
-      </c>
-      <c r="AI24" t="s">
-        <v>51</v>
-      </c>
-      <c r="AJ24" t="s">
-        <v>51</v>
-      </c>
-      <c r="AK24" t="s">
-        <v>51</v>
-      </c>
-      <c r="AL24" t="s">
-        <v>51</v>
-      </c>
-      <c r="AM24" t="s">
-        <v>51</v>
-      </c>
-      <c r="AO24" t="s">
-        <v>51</v>
-      </c>
-      <c r="AP24" t="s">
-        <v>51</v>
-      </c>
-      <c r="AQ24" t="s">
-        <v>51</v>
-      </c>
-      <c r="AR24" t="s">
-        <v>51</v>
-      </c>
-      <c r="AS24" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="25" spans="1:45">
       <c r="A25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B25" t="s">
         <v>55</v>
       </c>
-      <c r="D25" t="s">
-        <v>70</v>
-      </c>
-      <c r="F25" t="n">
-        <v>0</v>
-      </c>
-      <c r="G25" t="n">
-        <v>1</v>
-      </c>
-      <c r="H25" t="n">
-        <v>0</v>
-      </c>
-      <c r="I25" t="n">
-        <v>0</v>
-      </c>
-      <c r="L25" t="n">
-        <v>6</v>
-      </c>
-      <c r="M25" t="n">
-        <v>1</v>
-      </c>
-      <c r="N25" t="n">
-        <v>1</v>
-      </c>
-      <c r="O25" t="n">
-        <v>3</v>
-      </c>
-      <c r="R25" t="n">
-        <v>0</v>
-      </c>
-      <c r="S25" t="n">
-        <v>0</v>
-      </c>
-      <c r="T25" t="n">
-        <v>0</v>
-      </c>
-      <c r="U25" t="n">
-        <v>0</v>
-      </c>
-      <c r="X25" t="n">
-        <v>13</v>
-      </c>
-      <c r="Y25" t="n">
-        <v>6</v>
-      </c>
-      <c r="Z25" t="n">
-        <v>4</v>
-      </c>
-      <c r="AA25" t="n">
-        <v>5</v>
-      </c>
-      <c r="AD25" t="s">
-        <v>51</v>
-      </c>
-      <c r="AE25" t="s">
-        <v>51</v>
-      </c>
-      <c r="AF25" t="s">
-        <v>51</v>
-      </c>
-      <c r="AG25" t="s">
-        <v>51</v>
-      </c>
-      <c r="AJ25" t="s">
-        <v>51</v>
-      </c>
-      <c r="AK25" t="s">
-        <v>51</v>
-      </c>
-      <c r="AL25" t="s">
-        <v>51</v>
-      </c>
-      <c r="AM25" t="s">
-        <v>51</v>
-      </c>
-      <c r="AP25" t="s">
-        <v>51</v>
-      </c>
-      <c r="AQ25" t="s">
-        <v>51</v>
-      </c>
-      <c r="AR25" t="s">
-        <v>51</v>
-      </c>
-      <c r="AS25" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="26" spans="1:45">
       <c r="A26" t="s">
+        <v>74</v>
+      </c>
+      <c r="B26" t="s">
         <v>75</v>
-      </c>
-      <c r="B26" t="s">
-        <v>76</v>
-      </c>
-      <c r="D26" t="s">
-        <v>70</v>
-      </c>
-      <c r="G26" t="n">
-        <v>13</v>
-      </c>
-      <c r="H26" t="n">
-        <v>0</v>
-      </c>
-      <c r="I26" t="n">
-        <v>0</v>
-      </c>
-      <c r="M26" t="n">
-        <v>3</v>
-      </c>
-      <c r="N26" t="n">
-        <v>4</v>
-      </c>
-      <c r="O26" t="n">
-        <v>5</v>
-      </c>
-      <c r="S26" t="n">
-        <v>0</v>
-      </c>
-      <c r="T26" t="n">
-        <v>0</v>
-      </c>
-      <c r="U26" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y26" t="n">
-        <v>9</v>
-      </c>
-      <c r="Z26" t="n">
-        <v>12</v>
-      </c>
-      <c r="AA26" t="n">
-        <v>9</v>
-      </c>
-      <c r="AE26" t="s">
-        <v>51</v>
-      </c>
-      <c r="AF26" t="s">
-        <v>51</v>
-      </c>
-      <c r="AG26" t="s">
-        <v>51</v>
-      </c>
-      <c r="AK26" t="s">
-        <v>51</v>
-      </c>
-      <c r="AL26" t="s">
-        <v>51</v>
-      </c>
-      <c r="AM26" t="s">
-        <v>51</v>
-      </c>
-      <c r="AQ26" t="s">
-        <v>51</v>
-      </c>
-      <c r="AR26" t="s">
-        <v>51</v>
-      </c>
-      <c r="AS26" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:45">
       <c r="A27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B27" t="s">
         <v>55</v>
@@ -59379,7 +58933,7 @@
     </row>
     <row r="28" spans="1:45">
       <c r="A28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B28" t="s">
         <v>55</v>
@@ -59387,7 +58941,7 @@
     </row>
     <row r="29" spans="1:45">
       <c r="A29" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B29" t="s">
         <v>49</v>
@@ -59395,7 +58949,7 @@
     </row>
     <row r="30" spans="1:45">
       <c r="A30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B30" t="s">
         <v>49</v>
@@ -59403,7 +58957,7 @@
     </row>
     <row r="31" spans="1:45">
       <c r="A31" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B31" t="s">
         <v>49</v>
@@ -59411,7 +58965,7 @@
     </row>
     <row r="32" spans="1:45">
       <c r="A32" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B32" t="s">
         <v>55</v>
@@ -59419,7 +58973,7 @@
     </row>
     <row r="33" spans="1:45">
       <c r="A33" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B33" t="s">
         <v>55</v>
@@ -59427,7 +58981,7 @@
     </row>
     <row r="34" spans="1:45">
       <c r="A34" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B34" t="s">
         <v>55</v>
@@ -59435,7 +58989,7 @@
     </row>
     <row r="35" spans="1:45">
       <c r="A35" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B35" t="s">
         <v>49</v>
@@ -59443,7 +58997,7 @@
     </row>
     <row r="36" spans="1:45">
       <c r="A36" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B36" t="s">
         <v>61</v>
@@ -59559,7 +59113,7 @@
     </row>
     <row r="37" spans="1:45">
       <c r="A37" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B37" t="s">
         <v>49</v>
@@ -59675,7 +59229,7 @@
     </row>
     <row r="38" spans="1:45">
       <c r="A38" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B38" t="s">
         <v>49</v>
@@ -59683,7 +59237,7 @@
     </row>
     <row r="39" spans="1:45">
       <c r="A39" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B39" t="s">
         <v>49</v>
@@ -59691,7 +59245,7 @@
     </row>
     <row r="40" spans="1:45">
       <c r="A40" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B40" t="s">
         <v>61</v>
@@ -59702,7 +59256,7 @@
     </row>
     <row r="41" spans="1:45">
       <c r="A41" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B41" t="s">
         <v>49</v>
@@ -59710,7 +59264,7 @@
     </row>
     <row r="42" spans="1:45">
       <c r="A42" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B42" t="s">
         <v>49</v>
@@ -59718,7 +59272,7 @@
     </row>
     <row r="43" spans="1:45">
       <c r="A43" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B43" t="s">
         <v>49</v>
@@ -59726,7 +59280,7 @@
     </row>
     <row r="44" spans="1:45">
       <c r="A44" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B44" t="s">
         <v>61</v>
@@ -59842,7 +59396,7 @@
     </row>
     <row r="45" spans="1:45">
       <c r="A45" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B45" t="s">
         <v>49</v>
@@ -59850,7 +59404,7 @@
     </row>
     <row r="46" spans="1:45">
       <c r="A46" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B46" t="s">
         <v>55</v>
@@ -59966,7 +59520,7 @@
     </row>
     <row r="47" spans="1:45">
       <c r="A47" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B47" t="s">
         <v>49</v>
@@ -60082,7 +59636,7 @@
     </row>
     <row r="48" spans="1:45">
       <c r="A48" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B48" t="s">
         <v>55</v>
@@ -60090,7 +59644,7 @@
     </row>
     <row r="49" spans="1:45">
       <c r="A49" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B49" t="s">
         <v>49</v>
@@ -60206,7 +59760,7 @@
     </row>
     <row r="50" spans="1:45">
       <c r="A50" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B50" t="s">
         <v>55</v>
@@ -60322,7 +59876,7 @@
     </row>
     <row r="51" spans="1:45">
       <c r="A51" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B51" t="s">
         <v>49</v>
@@ -60330,7 +59884,7 @@
     </row>
     <row r="52" spans="1:45">
       <c r="A52" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B52" t="s">
         <v>55</v>
@@ -60338,7 +59892,7 @@
     </row>
     <row r="53" spans="1:45">
       <c r="A53" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B53" t="s">
         <v>49</v>
@@ -60454,7 +60008,7 @@
     </row>
     <row r="54" spans="1:45">
       <c r="A54" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B54" t="s">
         <v>49</v>
@@ -60570,7 +60124,7 @@
     </row>
     <row r="55" spans="1:45">
       <c r="A55" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B55" t="s">
         <v>61</v>
@@ -60578,7 +60132,7 @@
     </row>
     <row r="56" spans="1:45">
       <c r="A56" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B56" t="s">
         <v>49</v>
@@ -60694,7 +60248,7 @@
     </row>
     <row r="57" spans="1:45">
       <c r="A57" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B57" t="s">
         <v>49</v>
@@ -60810,7 +60364,7 @@
     </row>
     <row r="58" spans="1:45">
       <c r="A58" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B58" t="s">
         <v>55</v>
@@ -60818,10 +60372,10 @@
     </row>
     <row r="59" spans="1:45">
       <c r="A59" t="s">
+        <v>108</v>
+      </c>
+      <c r="B59" t="s">
         <v>109</v>
-      </c>
-      <c r="B59" t="s">
-        <v>110</v>
       </c>
       <c r="D59" t="s">
         <v>50</v>
@@ -60934,7 +60488,7 @@
     </row>
     <row r="60" spans="1:45">
       <c r="A60" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B60" t="s">
         <v>49</v>
@@ -60942,7 +60496,7 @@
     </row>
     <row r="61" spans="1:45">
       <c r="A61" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B61" t="s">
         <v>49</v>
@@ -60950,7 +60504,7 @@
     </row>
     <row r="62" spans="1:45">
       <c r="A62" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B62" t="s">
         <v>55</v>
@@ -60958,7 +60512,7 @@
     </row>
     <row r="63" spans="1:45">
       <c r="A63" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B63" t="s">
         <v>49</v>
@@ -60966,13 +60520,13 @@
     </row>
     <row r="64" spans="1:45">
       <c r="A64" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B64" t="s">
         <v>55</v>
       </c>
       <c r="D64" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E64" t="n">
         <v>0</v>
@@ -61082,13 +60636,13 @@
     </row>
     <row r="65" spans="1:45">
       <c r="A65" t="s">
+        <v>116</v>
+      </c>
+      <c r="B65" t="s">
         <v>117</v>
       </c>
-      <c r="B65" t="s">
-        <v>118</v>
-      </c>
       <c r="D65" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E65" t="n">
         <v>1</v>
@@ -61177,13 +60731,13 @@
     </row>
     <row r="66" spans="1:45">
       <c r="A66" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B66" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D66" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E66" t="n">
         <v>0</v>
@@ -61293,13 +60847,13 @@
     </row>
     <row r="67" spans="1:45">
       <c r="A67" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B67" t="s">
         <v>55</v>
       </c>
       <c r="D67" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E67" t="n">
         <v>0</v>
@@ -61388,13 +60942,13 @@
     </row>
     <row r="68" spans="1:45">
       <c r="A68" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B68" t="s">
         <v>55</v>
       </c>
       <c r="D68" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E68" t="n">
         <v>1</v>
@@ -61504,7 +61058,7 @@
     </row>
     <row r="69" spans="1:45">
       <c r="A69" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B69" t="s">
         <v>55</v>
@@ -61512,7 +61066,7 @@
     </row>
     <row r="70" spans="1:45">
       <c r="A70" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B70" t="s">
         <v>55</v>
@@ -61523,7 +61077,7 @@
     </row>
     <row r="71" spans="1:45">
       <c r="A71" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B71" t="s">
         <v>49</v>
@@ -61531,7 +61085,7 @@
     </row>
     <row r="72" spans="1:45">
       <c r="A72" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B72" t="s">
         <v>55</v>
@@ -61539,7 +61093,7 @@
     </row>
     <row r="73" spans="1:45">
       <c r="A73" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B73" t="s">
         <v>49</v>
@@ -61547,7 +61101,7 @@
     </row>
     <row r="74" spans="1:45">
       <c r="A74" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B74" t="s">
         <v>49</v>
@@ -61555,7 +61109,7 @@
     </row>
     <row r="75" spans="1:45">
       <c r="A75" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B75" t="s">
         <v>49</v>
@@ -61563,7 +61117,7 @@
     </row>
     <row r="76" spans="1:45">
       <c r="A76" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B76" t="s">
         <v>49</v>
@@ -61571,7 +61125,7 @@
     </row>
     <row r="77" spans="1:45">
       <c r="A77" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B77" t="s">
         <v>49</v>
@@ -61579,7 +61133,7 @@
     </row>
     <row r="78" spans="1:45">
       <c r="A78" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B78" t="s">
         <v>49</v>
@@ -61587,15 +61141,15 @@
     </row>
     <row r="79" spans="1:45">
       <c r="A79" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B79" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="80" spans="1:45">
       <c r="A80" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B80" t="s">
         <v>49</v>
@@ -61603,7 +61157,7 @@
     </row>
     <row r="81" spans="1:45">
       <c r="A81" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B81" t="s">
         <v>55</v>
@@ -61611,13 +61165,13 @@
     </row>
     <row r="82" spans="1:45">
       <c r="A82" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B82" t="s">
         <v>55</v>
       </c>
       <c r="D82" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E82" t="n">
         <v>1</v>
@@ -61727,13 +61281,13 @@
     </row>
     <row r="83" spans="1:45">
       <c r="A83" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B83" t="s">
         <v>49</v>
       </c>
       <c r="D83" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E83" t="n">
         <v>2</v>
@@ -61843,15 +61397,15 @@
     </row>
     <row r="84" spans="1:45">
       <c r="A84" t="s">
+        <v>137</v>
+      </c>
+      <c r="B84" t="s">
         <v>138</v>
-      </c>
-      <c r="B84" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="85" spans="1:45">
       <c r="A85" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B85" t="s">
         <v>55</v>
@@ -61859,13 +61413,13 @@
     </row>
     <row r="86" spans="1:45">
       <c r="A86" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B86" t="s">
         <v>49</v>
       </c>
       <c r="D86" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E86" t="n">
         <v>0</v>
@@ -61975,7 +61529,7 @@
     </row>
     <row r="87" spans="1:45">
       <c r="A87" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B87" t="s">
         <v>55</v>
@@ -61983,13 +61537,13 @@
     </row>
     <row r="88" spans="1:45">
       <c r="A88" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B88" t="s">
         <v>55</v>
       </c>
       <c r="D88" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E88" t="n">
         <v>0</v>
@@ -62099,13 +61653,13 @@
     </row>
     <row r="89" spans="1:45">
       <c r="A89" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B89" t="s">
         <v>49</v>
       </c>
       <c r="D89" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E89" t="n">
         <v>0</v>
@@ -62215,13 +61769,13 @@
     </row>
     <row r="90" spans="1:45">
       <c r="A90" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B90" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D90" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E90" t="n">
         <v>0</v>
@@ -62331,7 +61885,7 @@
     </row>
     <row r="91" spans="1:45">
       <c r="A91" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B91" t="s">
         <v>55</v>
@@ -62339,13 +61893,13 @@
     </row>
     <row r="92" spans="1:45">
       <c r="A92" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B92" t="s">
         <v>49</v>
       </c>
       <c r="D92" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E92" t="n">
         <v>4</v>
@@ -62455,21 +62009,21 @@
     </row>
     <row r="93" spans="1:45">
       <c r="A93" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B93" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="94" spans="1:45">
       <c r="A94" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B94" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D94" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E94" t="n">
         <v>2</v>
@@ -62579,13 +62133,13 @@
     </row>
     <row r="95" spans="1:45">
       <c r="A95" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B95" t="s">
         <v>49</v>
       </c>
       <c r="D95" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E95" t="n">
         <v>3</v>
@@ -62695,7 +62249,7 @@
     </row>
     <row r="96" spans="1:45">
       <c r="A96" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B96" t="s">
         <v>49</v>
@@ -62703,13 +62257,13 @@
     </row>
     <row r="97" spans="1:45">
       <c r="A97" t="s">
+        <v>151</v>
+      </c>
+      <c r="B97" t="s">
         <v>152</v>
       </c>
-      <c r="B97" t="s">
-        <v>153</v>
-      </c>
       <c r="D97" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E97" t="n">
         <v>0</v>
@@ -62819,13 +62373,13 @@
     </row>
     <row r="98" spans="1:45">
       <c r="A98" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B98" t="s">
         <v>49</v>
       </c>
       <c r="D98" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E98" t="n">
         <v>2</v>
@@ -62935,7 +62489,7 @@
     </row>
     <row r="99" spans="1:45">
       <c r="A99" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B99" t="s">
         <v>55</v>
@@ -62943,13 +62497,13 @@
     </row>
     <row r="100" spans="1:45">
       <c r="A100" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B100" t="s">
         <v>49</v>
       </c>
       <c r="D100" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E100" t="n">
         <v>0</v>
@@ -63059,13 +62613,13 @@
     </row>
     <row r="101" spans="1:45">
       <c r="A101" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B101" t="s">
         <v>55</v>
       </c>
       <c r="D101" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E101" t="n">
         <v>3</v>
@@ -63175,7 +62729,7 @@
     </row>
     <row r="102" spans="1:45">
       <c r="A102" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B102" t="s">
         <v>49</v>
@@ -63183,7 +62737,7 @@
     </row>
     <row r="103" spans="1:45">
       <c r="A103" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B103" t="s">
         <v>55</v>
@@ -63191,7 +62745,7 @@
     </row>
     <row r="104" spans="1:45">
       <c r="A104" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B104" t="s">
         <v>49</v>
@@ -63199,7 +62753,7 @@
     </row>
     <row r="105" spans="1:45">
       <c r="A105" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B105" t="s">
         <v>49</v>
@@ -63207,13 +62761,13 @@
     </row>
     <row r="106" spans="1:45">
       <c r="A106" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B106" t="s">
         <v>55</v>
       </c>
       <c r="D106" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E106" t="n">
         <v>2</v>
@@ -63323,13 +62877,13 @@
     </row>
     <row r="107" spans="1:45">
       <c r="A107" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B107" t="s">
         <v>61</v>
       </c>
       <c r="D107" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E107" t="n">
         <v>0</v>
@@ -63439,13 +62993,13 @@
     </row>
     <row r="108" spans="1:45">
       <c r="A108" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B108" t="s">
         <v>55</v>
       </c>
       <c r="D108" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E108" t="n">
         <v>0</v>
@@ -63555,13 +63109,13 @@
     </row>
     <row r="109" spans="1:45">
       <c r="A109" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B109" t="s">
         <v>49</v>
       </c>
       <c r="D109" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E109" t="n">
         <v>1</v>
@@ -63671,7 +63225,7 @@
     </row>
     <row r="110" spans="1:45">
       <c r="A110" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B110" t="s">
         <v>55</v>
@@ -63679,13 +63233,13 @@
     </row>
     <row r="111" spans="1:45">
       <c r="A111" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B111" t="s">
         <v>55</v>
       </c>
       <c r="D111" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E111" t="n">
         <v>2</v>
@@ -63795,13 +63349,13 @@
     </row>
     <row r="112" spans="1:45">
       <c r="A112" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B112" t="s">
         <v>55</v>
       </c>
       <c r="D112" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E112" t="n">
         <v>3</v>
@@ -63911,13 +63465,13 @@
     </row>
     <row r="113" spans="1:45">
       <c r="A113" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B113" t="s">
         <v>55</v>
       </c>
       <c r="D113" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E113" t="n">
         <v>0</v>
@@ -64027,13 +63581,13 @@
     </row>
     <row r="114" spans="1:45">
       <c r="A114" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B114" t="s">
         <v>55</v>
       </c>
       <c r="D114" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E114" t="n">
         <v>4</v>
@@ -64143,13 +63697,13 @@
     </row>
     <row r="115" spans="1:45">
       <c r="A115" t="s">
+        <v>171</v>
+      </c>
+      <c r="B115" t="s">
         <v>172</v>
       </c>
-      <c r="B115" t="s">
-        <v>173</v>
-      </c>
       <c r="D115" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E115" t="n">
         <v>12</v>
@@ -64259,13 +63813,13 @@
     </row>
     <row r="116" spans="1:45">
       <c r="A116" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B116" t="s">
         <v>55</v>
       </c>
       <c r="D116" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E116" t="n">
         <v>13</v>
@@ -64375,13 +63929,13 @@
     </row>
     <row r="117" spans="1:45">
       <c r="A117" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B117" t="s">
         <v>55</v>
       </c>
       <c r="D117" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E117" t="n">
         <v>2</v>
@@ -64491,13 +64045,13 @@
     </row>
     <row r="118" spans="1:45">
       <c r="A118" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B118" t="s">
         <v>49</v>
       </c>
       <c r="D118" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E118" t="n">
         <v>4</v>
@@ -64607,13 +64161,13 @@
     </row>
     <row r="119" spans="1:45">
       <c r="A119" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B119" t="s">
         <v>55</v>
       </c>
       <c r="D119" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E119" t="n">
         <v>2</v>
@@ -64723,13 +64277,13 @@
     </row>
     <row r="120" spans="1:45">
       <c r="A120" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B120" t="s">
         <v>55</v>
       </c>
       <c r="D120" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E120" t="n">
         <v>6</v>
@@ -64839,13 +64393,13 @@
     </row>
     <row r="121" spans="1:45">
       <c r="A121" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B121" t="s">
         <v>49</v>
       </c>
       <c r="D121" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E121" t="n">
         <v>4</v>
@@ -64955,13 +64509,13 @@
     </row>
     <row r="122" spans="1:45">
       <c r="A122" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B122" t="s">
         <v>49</v>
       </c>
       <c r="D122" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E122" t="n">
         <v>6</v>
@@ -65071,13 +64625,13 @@
     </row>
     <row r="123" spans="1:45">
       <c r="A123" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B123" t="s">
         <v>49</v>
       </c>
       <c r="D123" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E123" t="n">
         <v>8</v>
@@ -65187,123 +64741,18 @@
     </row>
     <row r="124" spans="1:45">
       <c r="A124" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B124" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="125" spans="1:45">
       <c r="A125" t="s">
+        <v>182</v>
+      </c>
+      <c r="B125" t="s">
         <v>183</v>
-      </c>
-      <c r="B125" t="s">
-        <v>184</v>
-      </c>
-      <c r="D125" t="s">
-        <v>185</v>
-      </c>
-      <c r="E125" t="n">
-        <v>1</v>
-      </c>
-      <c r="F125" t="n">
-        <v>0</v>
-      </c>
-      <c r="G125" t="n">
-        <v>1</v>
-      </c>
-      <c r="H125" t="n">
-        <v>0</v>
-      </c>
-      <c r="I125" t="n">
-        <v>0</v>
-      </c>
-      <c r="K125" t="n">
-        <v>3</v>
-      </c>
-      <c r="L125" t="n">
-        <v>2</v>
-      </c>
-      <c r="M125" t="n">
-        <v>7</v>
-      </c>
-      <c r="N125" t="n">
-        <v>2</v>
-      </c>
-      <c r="O125" t="n">
-        <v>4</v>
-      </c>
-      <c r="Q125" t="n">
-        <v>0</v>
-      </c>
-      <c r="R125" t="n">
-        <v>0</v>
-      </c>
-      <c r="S125" t="n">
-        <v>0</v>
-      </c>
-      <c r="T125" t="n">
-        <v>0</v>
-      </c>
-      <c r="U125" t="n">
-        <v>0</v>
-      </c>
-      <c r="W125" t="n">
-        <v>6</v>
-      </c>
-      <c r="X125" t="n">
-        <v>4</v>
-      </c>
-      <c r="Y125" t="n">
-        <v>17</v>
-      </c>
-      <c r="Z125" t="n">
-        <v>10</v>
-      </c>
-      <c r="AA125" t="n">
-        <v>13</v>
-      </c>
-      <c r="AC125" t="s">
-        <v>51</v>
-      </c>
-      <c r="AD125" t="s">
-        <v>51</v>
-      </c>
-      <c r="AE125" t="s">
-        <v>52</v>
-      </c>
-      <c r="AF125" t="s">
-        <v>51</v>
-      </c>
-      <c r="AG125" t="s">
-        <v>51</v>
-      </c>
-      <c r="AI125" t="s">
-        <v>51</v>
-      </c>
-      <c r="AJ125" t="s">
-        <v>51</v>
-      </c>
-      <c r="AK125" t="s">
-        <v>51</v>
-      </c>
-      <c r="AL125" t="s">
-        <v>51</v>
-      </c>
-      <c r="AM125" t="s">
-        <v>51</v>
-      </c>
-      <c r="AO125" t="s">
-        <v>51</v>
-      </c>
-      <c r="AP125" t="s">
-        <v>51</v>
-      </c>
-      <c r="AQ125" t="s">
-        <v>51</v>
-      </c>
-      <c r="AR125" t="s">
-        <v>51</v>
       </c>
       <c r="AS125" t="s">
         <v>51</v>
@@ -65370,7 +64819,7 @@
       </c>
       <c r="C2" s="51" t="n"/>
       <c r="G2" s="19" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="J2" s="19" t="n"/>
       <c r="L2" s="19" t="n"/>
@@ -65382,7 +64831,7 @@
       <c r="O2" s="19" t="n"/>
       <c r="P2" s="19" t="n"/>
       <c r="Q2" s="19" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="R2" s="19" t="n"/>
       <c r="S2" s="19" t="n"/>
@@ -65397,7 +64846,7 @@
     </row>
     <row r="4" spans="1:39">
       <c r="A4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:39">
@@ -65411,13 +64860,13 @@
         <v>30</v>
       </c>
       <c r="W6" t="s">
+        <v>187</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>188</v>
+      </c>
+      <c r="AI6" t="s">
         <v>189</v>
-      </c>
-      <c r="AC6" t="s">
-        <v>190</v>
-      </c>
-      <c r="AI6" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="7" spans="1:39">
@@ -65526,7 +64975,7 @@
     </row>
     <row r="8" spans="1:39">
       <c r="A8" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B8" t="s">
         <v>49</v>
@@ -65534,7 +64983,7 @@
     </row>
     <row r="9" spans="1:39">
       <c r="A9" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B9" t="s">
         <v>55</v>
@@ -65542,7 +64991,7 @@
     </row>
     <row r="10" spans="1:39">
       <c r="A10" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B10" t="s">
         <v>49</v>
@@ -65550,7 +64999,7 @@
     </row>
     <row r="11" spans="1:39">
       <c r="A11" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B11" t="s">
         <v>55</v>
@@ -65558,13 +65007,13 @@
     </row>
     <row r="12" spans="1:39">
       <c r="A12" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B12" t="s">
         <v>49</v>
       </c>
       <c r="D12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E12" t="n">
         <v>1</v>
@@ -65627,45 +65076,45 @@
         <v>0</v>
       </c>
       <c r="AC12" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="AD12" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="AE12" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="AF12" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="AG12" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="AI12" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="AJ12" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="AK12" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="AL12" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="AM12" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13" spans="1:39">
       <c r="A13" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B13" t="s">
         <v>55</v>
       </c>
       <c r="D13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E13" t="n">
         <v>3</v>
@@ -65728,45 +65177,45 @@
         <v>0</v>
       </c>
       <c r="AC13" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="AD13" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="AE13" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="AF13" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="AG13" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="AI13" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="AJ13" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="AK13" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="AL13" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="AM13" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="14" spans="1:39">
       <c r="A14" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B14" t="s">
         <v>49</v>
       </c>
       <c r="D14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -65829,39 +65278,39 @@
         <v>0</v>
       </c>
       <c r="AC14" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="AD14" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="AE14" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="AF14" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="AG14" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="AI14" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="AJ14" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="AK14" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="AL14" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="AM14" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="15" spans="1:39">
       <c r="A15" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B15" t="s">
         <v>55</v>
@@ -65869,13 +65318,13 @@
     </row>
     <row r="16" spans="1:39">
       <c r="A16" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B16" t="s">
         <v>49</v>
       </c>
       <c r="D16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E16" t="n">
         <v>1</v>
@@ -65938,39 +65387,39 @@
         <v>0</v>
       </c>
       <c r="AC16" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="AD16" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="AE16" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="AF16" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="AG16" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="AI16" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="AJ16" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="AK16" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="AL16" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="AM16" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="17" spans="1:39">
       <c r="A17" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B17" t="s">
         <v>55</v>
@@ -65978,7 +65427,7 @@
     </row>
     <row r="18" spans="1:39">
       <c r="A18" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B18" t="s">
         <v>49</v>
@@ -66047,89 +65496,50 @@
         <v>0</v>
       </c>
       <c r="AC18" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="AD18" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="AE18" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="AF18" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="AG18" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="AI18" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="AJ18" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="AK18" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="AL18" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="AM18" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="19" spans="1:39">
       <c r="A19" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B19" t="s">
         <v>49</v>
       </c>
-      <c r="D19" t="s">
-        <v>70</v>
-      </c>
-      <c r="H19" t="n">
-        <v>2</v>
-      </c>
-      <c r="I19" t="n">
-        <v>1</v>
-      </c>
-      <c r="N19" t="n">
-        <v>3</v>
-      </c>
-      <c r="O19" t="n">
-        <v>11</v>
-      </c>
-      <c r="T19" t="n">
-        <v>1</v>
-      </c>
-      <c r="U19" t="n">
-        <v>2</v>
-      </c>
-      <c r="Z19" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA19" t="n">
-        <v>8</v>
-      </c>
-      <c r="AF19" t="s">
-        <v>206</v>
-      </c>
-      <c r="AG19" t="s">
-        <v>207</v>
-      </c>
-      <c r="AL19" t="s">
-        <v>208</v>
-      </c>
-      <c r="AM19" t="s">
-        <v>209</v>
-      </c>
     </row>
     <row r="20" spans="1:39">
       <c r="A20" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="D20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E20" t="n">
         <v>1</v>
@@ -66192,34 +65602,34 @@
         <v>0</v>
       </c>
       <c r="AC20" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="AD20" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="AE20" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="AF20" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="AG20" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="AI20" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="AJ20" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="AK20" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="AL20" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="AM20" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>